<commit_message>
update push for ugerm
</commit_message>
<xml_diff>
--- a/resources/GAS_M1_lineages.xlsx
+++ b/resources/GAS_M1_lineages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/data/tools/git.repositories/GeneSNPdetector/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E380E406-11F4-6B45-9BF9-507C9E78A667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3989FD23-716A-C04A-BE0B-AD02DF706664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9520" yWindow="3900" windowWidth="27640" windowHeight="16940" xr2:uid="{92912364-4034-6448-B943-36E2A2D04D60}"/>
   </bookViews>
@@ -47,12 +47,6 @@
     <t>position</t>
   </si>
   <si>
-    <t>ref_base</t>
-  </si>
-  <si>
-    <t>alt_base</t>
-  </si>
-  <si>
     <t>notes</t>
   </si>
   <si>
@@ -207,6 +201,12 @@
   </si>
   <si>
     <t>level</t>
+  </si>
+  <si>
+    <t>ref</t>
+  </si>
+  <si>
+    <t>alt</t>
   </si>
 </sst>
 </file>
@@ -561,7 +561,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B37"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -574,28 +574,28 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
       <c r="H1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -603,851 +603,851 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C2">
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C3">
         <v>954</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
         <v>16</v>
       </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
       <c r="I3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C4">
         <v>955</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
         <v>16</v>
       </c>
-      <c r="H4" t="s">
-        <v>18</v>
-      </c>
       <c r="I4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C5">
         <v>1471</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" t="s">
         <v>15</v>
-      </c>
-      <c r="F5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C6">
         <v>744</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C7">
         <v>346</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C8">
         <v>154</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C9">
         <v>899</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C10">
         <v>130</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C11">
         <v>1007</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C12">
         <v>441</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C13">
         <v>244</v>
       </c>
       <c r="D13" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C14">
         <v>302</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C15">
         <v>367</v>
       </c>
       <c r="D15" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C16">
         <v>661</v>
       </c>
       <c r="D16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C17">
         <v>95</v>
       </c>
       <c r="D17" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E17" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G17" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C18">
         <v>212</v>
       </c>
       <c r="D18" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C19">
         <v>404</v>
       </c>
       <c r="D19" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G19" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C20">
         <v>198</v>
       </c>
       <c r="D20" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E20" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G20" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B21" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C21">
         <v>693</v>
       </c>
       <c r="D21" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E21" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F21" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G21" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C22">
         <v>524</v>
       </c>
       <c r="D22" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E22" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F22" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G22" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C23">
         <v>181</v>
       </c>
       <c r="D23" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E23" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F23" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G23" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C24">
         <v>889</v>
       </c>
       <c r="D24" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E24" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F24" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G24" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C25">
         <v>683</v>
       </c>
       <c r="D25" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E25" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C26">
         <v>442</v>
       </c>
       <c r="D26" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E26" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F26" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G26" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C27">
         <v>336</v>
       </c>
       <c r="D27" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E27" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F27" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B28" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C28">
         <v>729</v>
       </c>
       <c r="D28" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E28" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F28" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G28" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C29">
         <v>57</v>
       </c>
       <c r="D29" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E29" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F29" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C30">
         <v>43</v>
       </c>
       <c r="D30" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E30" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F30" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G30" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B31" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C31">
         <v>417</v>
       </c>
       <c r="D31" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E31" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F31" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G31" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B32" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C32">
         <v>908</v>
       </c>
       <c r="D32" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E32" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F32" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G32" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B33" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C33">
         <v>1318</v>
       </c>
       <c r="D33" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E33" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F33" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G33" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B34" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C34">
         <v>397</v>
       </c>
       <c r="D34" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E34" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F34" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G34" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B35" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C35">
         <v>76</v>
       </c>
       <c r="D35" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E35" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F35" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G35" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B36" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C36">
         <v>260</v>
       </c>
       <c r="D36" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E36" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F36" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G36" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B37" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C37">
         <v>291</v>
       </c>
       <c r="D37" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E37" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F37" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G37" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>